<commit_message>
Login added negative Testcases
</commit_message>
<xml_diff>
--- a/mmpequinox/mmpdata.xlsx
+++ b/mmpequinox/mmpdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\eclipse-workspace\IITWF2025\mmpequinox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zz96jl/git/equinoxmmp/mmpequinox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26315EF1-5492-4AE9-A916-BECFDDC54C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6906EDC7-FCE0-8A40-AD04-6CBBB76F407A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{400A5CF3-F14E-4052-9EDB-0C9330A1317C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{400A5CF3-F14E-4052-9EDB-0C9330A1317C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>ria1</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Ria112135135</t>
+  </si>
+  <si>
+    <t>Ria123456</t>
+  </si>
+  <si>
+    <t>ria12</t>
   </si>
 </sst>
 </file>
@@ -92,9 +98,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -132,7 +138,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -238,7 +244,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -380,7 +386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -388,55 +394,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FCED7E-256D-48A8-B936-407E57BB5A72}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>123456</v>
-      </c>
-      <c r="B5">
-        <v>125151521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Listener details in the suite.xml
</commit_message>
<xml_diff>
--- a/mmpequinox/mmpdata.xlsx
+++ b/mmpequinox/mmpdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\eclipse-workspace\IITWF2025\mmpequinox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\equinoxmmp1\mmpequinox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26315EF1-5492-4AE9-A916-BECFDDC54C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB23DBF-C7FA-46CD-8860-30FC7A7FD6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{400A5CF3-F14E-4052-9EDB-0C9330A1317C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{400A5CF3-F14E-4052-9EDB-0C9330A1317C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ria1</t>
   </si>
   <si>
     <t>Ria12345</t>
-  </si>
-  <si>
-    <t>ria2</t>
-  </si>
-  <si>
-    <t>Ria112135135</t>
   </si>
 </sst>
 </file>
@@ -388,11 +382,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FCED7E-256D-48A8-B936-407E57BB5A72}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -407,38 +399,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>123456</v>
-      </c>
-      <c r="B5">
-        <v>125151521</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>